<commit_message>
Atualização automática - 24/02/2026 09:28
</commit_message>
<xml_diff>
--- a/dados/ENTREGAS_DIA.xlsx
+++ b/dados/ENTREGAS_DIA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Dashboard_Sauipe\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F32F73B-20BA-4DA3-8329-706FE4BDBB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BECFE6-6D35-4409-8DEE-35944F46F5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,11 +566,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,12 +700,76 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2">
+        <v>46068</v>
+      </c>
+      <c r="B16">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>46069</v>
+      </c>
+      <c r="B17">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>46070</v>
+      </c>
+      <c r="B18">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>46071</v>
+      </c>
+      <c r="B19">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>46072</v>
+      </c>
+      <c r="B20">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>46073</v>
+      </c>
+      <c r="B21">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>46074</v>
+      </c>
+      <c r="B22">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>46075</v>
+      </c>
+      <c r="B23">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="5">
-        <f>SUM(B2:B15)</f>
-        <v>4665</v>
+      <c r="B24" s="5">
+        <f>SUM(B2:B23)</f>
+        <v>7327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>